<commit_message>
Completed regional data compilation incl. run size where available (output/sps-data.csv)
</commit_message>
<xml_diff>
--- a/data/E. Hertz - IFC Data.xlsx
+++ b/data/E. Hertz - IFC Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Data Management\Data Requests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephaniepeacock/Salmon Watersheds Dropbox/Stephanie Peacock/X Drive/1_PROJECTS/1_Active/State of Salmon/Data and Analysis/state-of-salmon/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA109B1-B6C7-4604-A3CD-E37E0F0371E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42378A34-3DF4-DE49-AC9C-62DC66215A3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{A7107DDD-10EC-4EE7-B1A8-BC942E037E6E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="21140" windowHeight="16480" activeTab="1" xr2:uid="{A7107DDD-10EC-4EE7-B1A8-BC942E037E6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" r:id="rId1"/>
@@ -223,7 +223,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -233,6 +233,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -329,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -342,21 +348,23 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -685,204 +693,204 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="94.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.453125" customWidth="1"/>
-    <col min="5" max="5" width="26.36328125" customWidth="1"/>
+    <col min="1" max="1" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="94.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="12" t="s">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="18" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="16" t="s">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="16"/>
+      <c r="B10" s="15"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="66.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:5" ht="66.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:5" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="41.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:5" ht="41.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -911,17 +919,17 @@
       <selection pane="bottomLeft" activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" customWidth="1"/>
-    <col min="2" max="2" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="21.26953125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" s="1" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -941,7 +949,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1984</v>
       </c>
@@ -962,7 +970,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1985</v>
       </c>
@@ -983,7 +991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1986</v>
       </c>
@@ -1004,7 +1012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1987</v>
       </c>
@@ -1025,7 +1033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1988</v>
       </c>
@@ -1046,7 +1054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1989</v>
       </c>
@@ -1067,7 +1075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1990</v>
       </c>
@@ -1088,7 +1096,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1991</v>
       </c>
@@ -1109,7 +1117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1992</v>
       </c>
@@ -1130,7 +1138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1993</v>
       </c>
@@ -1151,7 +1159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1994</v>
       </c>
@@ -1172,7 +1180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1995</v>
       </c>
@@ -1193,7 +1201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1996</v>
       </c>
@@ -1214,7 +1222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1997</v>
       </c>
@@ -1235,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1998</v>
       </c>
@@ -1256,7 +1264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1999</v>
       </c>
@@ -1277,7 +1285,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2000</v>
       </c>
@@ -1298,7 +1306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2001</v>
       </c>
@@ -1319,7 +1327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2002</v>
       </c>
@@ -1340,7 +1348,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2003</v>
       </c>
@@ -1361,7 +1369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2004</v>
       </c>
@@ -1382,7 +1390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2005</v>
       </c>
@@ -1403,7 +1411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2006</v>
       </c>
@@ -1424,7 +1432,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2007</v>
       </c>
@@ -1445,7 +1453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2008</v>
       </c>
@@ -1466,7 +1474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2009</v>
       </c>
@@ -1487,7 +1495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2010</v>
       </c>
@@ -1508,7 +1516,7 @@
         <v>0.22220683410978381</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2011</v>
       </c>
@@ -1529,7 +1537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2012</v>
       </c>
@@ -1550,7 +1558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2013</v>
       </c>
@@ -1571,7 +1579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2014</v>
       </c>
@@ -1592,7 +1600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2015</v>
       </c>
@@ -1613,7 +1621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2016</v>
       </c>
@@ -1634,7 +1642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2017</v>
       </c>
@@ -1655,7 +1663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2018</v>
       </c>
@@ -1676,7 +1684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2019</v>
       </c>
@@ -1697,7 +1705,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2020</v>
       </c>
@@ -1718,7 +1726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2021</v>
       </c>
@@ -1739,7 +1747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2022</v>
       </c>
@@ -1760,7 +1768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>1984</v>
       </c>
@@ -1781,7 +1789,7 @@
         <v>5.4159033340047245</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>1985</v>
       </c>
@@ -1802,7 +1810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>1986</v>
       </c>
@@ -1823,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1987</v>
       </c>
@@ -1844,7 +1852,7 @@
         <v>91.795026194419734</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>1988</v>
       </c>
@@ -1865,7 +1873,7 @@
         <v>1601.1880259480604</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1989</v>
       </c>
@@ -1886,7 +1894,7 @@
         <v>3381.6076226329342</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>1990</v>
       </c>
@@ -1907,7 +1915,7 @@
         <v>1625.3868377706785</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>1991</v>
       </c>
@@ -1928,7 +1936,7 @@
         <v>1753.3968095924993</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1992</v>
       </c>
@@ -1949,7 +1957,7 @@
         <v>2501.0617365632415</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>1993</v>
       </c>
@@ -1970,7 +1978,7 @@
         <v>1843.6262340615922</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>1994</v>
       </c>
@@ -1991,7 +1999,7 @@
         <v>5272.1425302271982</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>1995</v>
       </c>
@@ -2012,7 +2020,7 @@
         <v>47.292594239019309</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>1996</v>
       </c>
@@ -2033,7 +2041,7 @@
         <v>864.57538997849883</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>1997</v>
       </c>
@@ -2054,7 +2062,7 @@
         <v>1635.9414871105591</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>1998</v>
       </c>
@@ -2075,7 +2083,7 @@
         <v>2034.0388957280334</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1999</v>
       </c>
@@ -2096,7 +2104,7 @@
         <v>2787.1827655669699</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2000</v>
       </c>
@@ -2117,7 +2125,7 @@
         <v>2760.3276364692802</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2001</v>
       </c>
@@ -2138,7 +2146,7 @@
         <v>5117.8871710515186</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2002</v>
       </c>
@@ -2159,7 +2167,7 @@
         <v>10586.023309767672</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2003</v>
       </c>
@@ -2180,7 +2188,7 @@
         <v>1354.3295224550111</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>2004</v>
       </c>
@@ -2201,7 +2209,7 @@
         <v>1694.8926743156444</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2005</v>
       </c>
@@ -2222,7 +2230,7 @@
         <v>768.61975727254685</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>2006</v>
       </c>
@@ -2243,7 +2251,7 @@
         <v>19.057303329389015</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>2007</v>
       </c>
@@ -2264,7 +2272,7 @@
         <v>1206.0461520420995</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2008</v>
       </c>
@@ -2285,7 +2293,7 @@
         <v>405.08857461267507</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2009</v>
       </c>
@@ -2306,7 +2314,7 @@
         <v>955.25551730842699</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2010</v>
       </c>
@@ -2327,7 +2335,7 @@
         <v>1059.8548514408194</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2011</v>
       </c>
@@ -2348,7 +2356,7 @@
         <v>913.40200917513994</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2012</v>
       </c>
@@ -2369,7 +2377,7 @@
         <v>1016.3314283190412</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2013</v>
       </c>
@@ -2390,7 +2398,7 @@
         <v>584.91356361872931</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>2014</v>
       </c>
@@ -2411,7 +2419,7 @@
         <v>1029.3002257722401</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2015</v>
       </c>
@@ -2432,7 +2440,7 @@
         <v>620.66525502481909</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2016</v>
       </c>
@@ -2453,7 +2461,7 @@
         <v>1000.1658563734854</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2017</v>
       </c>
@@ -2474,7 +2482,7 @@
         <v>583.37292078314431</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2018</v>
       </c>
@@ -2495,7 +2503,7 @@
         <v>622.77215323605651</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2019</v>
       </c>
@@ -2516,7 +2524,7 @@
         <v>2388.7141656338226</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>2020</v>
       </c>
@@ -2537,7 +2545,7 @@
         <v>3297.0303634803804</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>2021</v>
       </c>
@@ -2558,7 +2566,7 @@
         <v>6528.2276859020349</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>2022</v>
       </c>
@@ -2579,7 +2587,7 @@
         <v>2024.7680344850523</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>1984</v>
       </c>
@@ -2600,7 +2608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>1985</v>
       </c>
@@ -2621,7 +2629,7 @@
         <v>166.9769129213455</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>1986</v>
       </c>
@@ -2642,7 +2650,7 @@
         <v>64.413989897886267</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>1987</v>
       </c>
@@ -2663,7 +2671,7 @@
         <v>0.24186563140483486</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>1988</v>
       </c>
@@ -2684,7 +2692,7 @@
         <v>56.928798913480023</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>1989</v>
       </c>
@@ -2705,7 +2713,7 @@
         <v>90.71120449072987</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>1990</v>
       </c>
@@ -2726,7 +2734,7 @@
         <v>40.982420328298758</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>1991</v>
       </c>
@@ -2747,7 +2755,7 @@
         <v>134.53030578585094</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>1992</v>
       </c>
@@ -2768,7 +2776,7 @@
         <v>85.908261602399762</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>1993</v>
       </c>
@@ -2789,7 +2797,7 @@
         <v>24.590797300915256</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>1994</v>
       </c>
@@ -2810,7 +2818,7 @@
         <v>0.5530832657150313</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>1995</v>
       </c>
@@ -2831,7 +2839,7 @@
         <v>24.708544554756827</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>1996</v>
       </c>
@@ -2852,7 +2860,7 @@
         <v>21.629541535794033</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>1997</v>
       </c>
@@ -2873,7 +2881,7 @@
         <v>11.445525173844089</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>1998</v>
       </c>
@@ -2894,7 +2902,7 @@
         <v>17.075422016710036</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>1999</v>
       </c>
@@ -2915,7 +2923,7 @@
         <v>43.731999480602099</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>2000</v>
       </c>
@@ -2936,7 +2944,7 @@
         <v>48.243558908622163</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>2001</v>
       </c>
@@ -2957,7 +2965,7 @@
         <v>278.02919399951861</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>2002</v>
       </c>
@@ -2978,7 +2986,7 @@
         <v>145.040224876921</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>2003</v>
       </c>
@@ -2999,7 +3007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>2004</v>
       </c>
@@ -3020,7 +3028,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>2005</v>
       </c>
@@ -3041,7 +3049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>2006</v>
       </c>
@@ -3062,7 +3070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>2007</v>
       </c>
@@ -3083,7 +3091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>2008</v>
       </c>
@@ -3104,7 +3112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>2009</v>
       </c>
@@ -3125,7 +3133,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>2010</v>
       </c>
@@ -3146,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>2011</v>
       </c>
@@ -3167,7 +3175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>2012</v>
       </c>
@@ -3188,7 +3196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>2013</v>
       </c>
@@ -3209,7 +3217,7 @@
         <v>9.1219390766382276</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>2014</v>
       </c>
@@ -3230,7 +3238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>2015</v>
       </c>
@@ -3251,7 +3259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>2016</v>
       </c>
@@ -3272,7 +3280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>2017</v>
       </c>
@@ -3293,7 +3301,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>2018</v>
       </c>
@@ -3314,7 +3322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>2019</v>
       </c>
@@ -3335,7 +3343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>2020</v>
       </c>
@@ -3356,7 +3364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>2021</v>
       </c>
@@ -3377,7 +3385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>2022</v>
       </c>
@@ -3398,7 +3406,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>1984</v>
       </c>
@@ -3419,7 +3427,7 @@
         <v>7.3885829614810064</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>1985</v>
       </c>
@@ -3440,7 +3448,7 @@
         <v>105.57810099718336</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>1986</v>
       </c>
@@ -3461,7 +3469,7 @@
         <v>461.68838811625028</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>1987</v>
       </c>
@@ -3482,7 +3490,7 @@
         <v>577.5068367872409</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>1988</v>
       </c>
@@ -3503,7 +3511,7 @@
         <v>1589.7957918521497</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>1989</v>
       </c>
@@ -3524,7 +3532,7 @@
         <v>1402.4164780935571</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>1990</v>
       </c>
@@ -3545,7 +3553,7 @@
         <v>996.09838948044853</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>1991</v>
       </c>
@@ -3566,7 +3574,7 @@
         <v>1604.281930118219</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>1992</v>
       </c>
@@ -3587,7 +3595,7 @@
         <v>1089.7213657368466</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>1993</v>
       </c>
@@ -3608,7 +3616,7 @@
         <v>335.5628121999689</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>1994</v>
       </c>
@@ -3629,7 +3637,7 @@
         <v>865.93691389560809</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>1995</v>
       </c>
@@ -3650,7 +3658,7 @@
         <v>242.71648835825363</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>1996</v>
       </c>
@@ -3671,7 +3679,7 @@
         <v>92.296545294572752</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>1997</v>
       </c>
@@ -3692,7 +3700,7 @@
         <v>694.13615601199581</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>1998</v>
       </c>
@@ -3713,7 +3721,7 @@
         <v>472.54198637634181</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>1999</v>
       </c>
@@ -3734,7 +3742,7 @@
         <v>211.91239510372543</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>2000</v>
       </c>
@@ -3755,7 +3763,7 @@
         <v>1589.7838161895406</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>2001</v>
       </c>
@@ -3776,7 +3784,7 @@
         <v>1811.3080792958644</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>2002</v>
       </c>
@@ -3797,7 +3805,7 @@
         <v>2484.8334605380405</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>2003</v>
       </c>
@@ -3818,7 +3826,7 @@
         <v>556.45837091069643</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>2004</v>
       </c>
@@ -3839,7 +3847,7 @@
         <v>449.54798521171324</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>2005</v>
       </c>
@@ -3860,7 +3868,7 @@
         <v>137.25359860832032</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>2006</v>
       </c>
@@ -3881,7 +3889,7 @@
         <v>6.605833929048913</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>2007</v>
       </c>
@@ -3902,7 +3910,7 @@
         <v>310.55776721176153</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>2008</v>
       </c>
@@ -3923,7 +3931,7 @@
         <v>199.69074363731443</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>2009</v>
       </c>
@@ -3944,7 +3952,7 @@
         <v>428.85561821410374</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>2010</v>
       </c>
@@ -3965,7 +3973,7 @@
         <v>501.18208055297146</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>2011</v>
       </c>
@@ -3986,7 +3994,7 @@
         <v>457.38273039578417</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>2012</v>
       </c>
@@ -4007,7 +4015,7 @@
         <v>598.03489734154937</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>2013</v>
       </c>
@@ -4028,7 +4036,7 @@
         <v>420.15111345964033</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>2014</v>
       </c>
@@ -4049,7 +4057,7 @@
         <v>68.240584242440491</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>2015</v>
       </c>
@@ -4070,7 +4078,7 @@
         <v>68.810067032324241</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>2016</v>
       </c>
@@ -4091,7 +4099,7 @@
         <v>109.46912269122913</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>2017</v>
       </c>
@@ -4112,7 +4120,7 @@
         <v>135.83766717324033</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>2018</v>
       </c>
@@ -4133,7 +4141,7 @@
         <v>208.83749990802062</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>2019</v>
       </c>
@@ -4154,7 +4162,7 @@
         <v>243.31267495690008</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>2020</v>
       </c>
@@ -4175,7 +4183,7 @@
         <v>350.89634440496957</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>2021</v>
       </c>
@@ -4196,7 +4204,7 @@
         <v>833.47845455805873</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>2022</v>
       </c>
@@ -4217,7 +4225,7 @@
         <v>371.6727943637743</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>1984</v>
       </c>
@@ -4238,7 +4246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>1985</v>
       </c>
@@ -4259,7 +4267,7 @@
         <v>0.24343622178275837</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>1986</v>
       </c>
@@ -4280,7 +4288,7 @@
         <v>1018.387731080802</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>1987</v>
       </c>
@@ -4301,7 +4309,7 @@
         <v>7099.9996259719155</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>1988</v>
       </c>
@@ -4322,7 +4330,7 @@
         <v>4704.4041902042154</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>1989</v>
       </c>
@@ -4343,7 +4351,7 @@
         <v>4520.1800823977774</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>1990</v>
       </c>
@@ -4364,7 +4372,7 @@
         <v>2717.5165396619941</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>1991</v>
       </c>
@@ -4385,7 +4393,7 @@
         <v>1979.1558514759499</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>1992</v>
       </c>
@@ -4406,7 +4414,7 @@
         <v>2260.1347185466984</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>1993</v>
       </c>
@@ -4427,7 +4435,7 @@
         <v>785.79802592607848</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>1994</v>
       </c>
@@ -4448,7 +4456,7 @@
         <v>876.25160989341293</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>1995</v>
       </c>
@@ -4469,7 +4477,7 @@
         <v>1070.1626633489718</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>1996</v>
       </c>
@@ -4490,7 +4498,7 @@
         <v>62.426745804841858</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>1997</v>
       </c>
@@ -4511,7 +4519,7 @@
         <v>16.282529079030382</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>1998</v>
       </c>
@@ -4532,7 +4540,7 @@
         <v>50.973610689553425</v>
       </c>
     </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>1999</v>
       </c>
@@ -4553,7 +4561,7 @@
         <v>56.07484796574181</v>
       </c>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>2000</v>
       </c>
@@ -4574,7 +4582,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>2001</v>
       </c>
@@ -4595,7 +4603,7 @@
         <v>1546.1953916362472</v>
       </c>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>2002</v>
       </c>
@@ -4616,7 +4624,7 @@
         <v>1570.6626424476599</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>2003</v>
       </c>
@@ -4637,7 +4645,7 @@
         <v>242.36960755619839</v>
       </c>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>2004</v>
       </c>
@@ -4658,7 +4666,7 @@
         <v>615.17064119839233</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>2005</v>
       </c>
@@ -4679,7 +4687,7 @@
         <v>370.78836760672812</v>
       </c>
     </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>2006</v>
       </c>
@@ -4700,7 +4708,7 @@
         <v>2.6098236658463065</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>2007</v>
       </c>
@@ -4721,7 +4729,7 @@
         <v>709.88133135025964</v>
       </c>
     </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>2008</v>
       </c>
@@ -4742,7 +4750,7 @@
         <v>375.48175494660245</v>
       </c>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>2009</v>
       </c>
@@ -4763,7 +4771,7 @@
         <v>174.67948718582602</v>
       </c>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>2010</v>
       </c>
@@ -4784,7 +4792,7 @@
         <v>613.71825878591881</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>2011</v>
       </c>
@@ -4805,7 +4813,7 @@
         <v>1105.0000000000005</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>2012</v>
       </c>
@@ -4826,7 +4834,7 @@
         <v>605.68617517791245</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>2013</v>
       </c>
@@ -4847,7 +4855,7 @@
         <v>1345.456666541977</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>2014</v>
       </c>
@@ -4868,7 +4876,7 @@
         <v>306.88325175912951</v>
       </c>
     </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>2015</v>
       </c>
@@ -4889,7 +4897,7 @@
         <v>538.60078941243182</v>
       </c>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>2016</v>
       </c>
@@ -4910,7 +4918,7 @@
         <v>1081.4270880588174</v>
       </c>
     </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>2017</v>
       </c>
@@ -4931,7 +4939,7 @@
         <v>557.86168937600041</v>
       </c>
     </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>2018</v>
       </c>
@@ -4952,7 +4960,7 @@
         <v>658.78457972622164</v>
       </c>
     </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>2019</v>
       </c>
@@ -4973,7 +4981,7 @@
         <v>601.42094118300975</v>
       </c>
     </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>2020</v>
       </c>
@@ -4994,7 +5002,7 @@
         <v>1870.0813120803014</v>
       </c>
     </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>2021</v>
       </c>
@@ -5015,7 +5023,7 @@
         <v>2941.8562405487246</v>
       </c>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>2022</v>
       </c>

</xml_diff>